<commit_message>
Added build, feeder change - still pre-beta
</commit_message>
<xml_diff>
--- a/hospitalConfig/hospitals/hospital1.xlsx
+++ b/hospitalConfig/hospitals/hospital1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/82cfe7acc6d68563/Documents/github/Clinical-Costing/hospitalConfig/hospitals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="358" documentId="8_{F21D1F19-B0D4-4D89-B817-A6C872BD26CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D4615FA-CF01-4720-B94F-CFE64B3C8821}"/>
+  <xr:revisionPtr revIDLastSave="361" documentId="8_{F21D1F19-B0D4-4D89-B817-A6C872BD26CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E71B043-7BB9-491E-8595-542EE9C8D18D}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="10" xr2:uid="{EE86B12F-8EEC-43A3-B99E-E677A24C294A}"/>
   </bookViews>
@@ -26,8 +26,8 @@
     <sheet name="feeders" sheetId="16" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="2" hidden="1">departments!$A$1:$B$62</definedName>
-    <definedName name="ExternalData_2" localSheetId="3" hidden="1">'cost types'!$A$1:$B$36</definedName>
+    <definedName name="ExternalData_1" localSheetId="2" hidden="1">departments!$A$1:$B$61</definedName>
+    <definedName name="ExternalData_2" localSheetId="3" hidden="1">'cost types'!$A$1:$B$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="344">
   <si>
     <t>ADMIN</t>
   </si>
@@ -1008,12 +1008,6 @@
     <t>Prosthetics Adjustment</t>
   </si>
   <si>
-    <t>No associated department</t>
-  </si>
-  <si>
-    <t>no associated cost type</t>
-  </si>
-  <si>
     <t>feeder_type_code</t>
   </si>
   <si>
@@ -1066,12 +1060,6 @@
   </si>
   <si>
     <t>prosthetic</t>
-  </si>
-  <si>
-    <t>new_department_code</t>
-  </si>
-  <si>
-    <t>new_cost_type_code</t>
   </si>
   <si>
     <t>prosth</t>
@@ -1234,8 +1222,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0EDF33CA-A7D8-4ADF-8495-B631FA268A25}" name="dept" displayName="dept" ref="A1:B62" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:B62" xr:uid="{0EDF33CA-A7D8-4ADF-8495-B631FA268A25}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0EDF33CA-A7D8-4ADF-8495-B631FA268A25}" name="dept" displayName="dept" ref="A1:B61" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:B61" xr:uid="{0EDF33CA-A7D8-4ADF-8495-B631FA268A25}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{618E4927-3164-4209-88C4-E051AFD98A74}" uniqueName="1" name="department_code" queryTableFieldId="1" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{2A824303-703D-4EA0-BADD-267AF6C35625}" uniqueName="2" name="department_name" queryTableFieldId="2" dataDxfId="2"/>
@@ -1245,8 +1233,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{49776610-1554-4112-BBD4-DBCAB5DF817C}" name="costtype" displayName="costtype" ref="A1:B36" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:B36" xr:uid="{49776610-1554-4112-BBD4-DBCAB5DF817C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{49776610-1554-4112-BBD4-DBCAB5DF817C}" name="costtype" displayName="costtype" ref="A1:B35" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:B35" xr:uid="{49776610-1554-4112-BBD4-DBCAB5DF817C}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{D3124862-DA24-43F5-BD00-523AC2BF7B5C}" uniqueName="1" name="cost_type_code" queryTableFieldId="1" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{56F2815C-D89C-4975-A98A-3B9679A67317}" uniqueName="2" name="cost_type_description" queryTableFieldId="2" dataDxfId="0"/>
@@ -1718,26 +1706,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -1747,156 +1735,118 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2057FB1-CD68-4671-BA7D-809E4713A0D4}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="10.578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.05078125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.20703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5234375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.5234375" customWidth="1"/>
-    <col min="7" max="7" width="29.7890625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.5234375" customWidth="1"/>
+    <col min="5" max="5" width="29.7890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D1" t="s">
+        <v>337</v>
+      </c>
+      <c r="E1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
         <v>323</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>317</v>
       </c>
-      <c r="C1" t="s">
-        <v>335</v>
-      </c>
-      <c r="D1" t="s">
-        <v>336</v>
-      </c>
-      <c r="E1" t="s">
-        <v>340</v>
-      </c>
-      <c r="F1" t="s">
-        <v>341</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="D2" s="3">
+        <v>8.1</v>
+      </c>
+      <c r="E2" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>325</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B3" t="s">
         <v>319</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" t="s">
-        <v>338</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="F2" s="3">
-        <v>8.1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>334</v>
-      </c>
-      <c r="B3" t="s">
-        <v>321</v>
       </c>
       <c r="C3" t="s">
         <v>271</v>
       </c>
-      <c r="D3" t="s">
-        <v>271</v>
-      </c>
       <c r="E3" t="s">
-        <v>271</v>
-      </c>
-      <c r="G3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>326</v>
+      </c>
+      <c r="B4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="D4" s="5">
+        <v>9.1</v>
+      </c>
+      <c r="E4" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
         <v>328</v>
       </c>
-      <c r="B4" t="s">
-        <v>319</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D4" t="s">
-        <v>338</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="F4" s="5">
-        <v>9.1</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="B5" t="s">
+        <v>317</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="D5" s="3">
+        <v>10.1</v>
+      </c>
+      <c r="E5" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
         <v>330</v>
       </c>
-      <c r="B5" t="s">
-        <v>319</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" t="s">
-        <v>338</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="F5" s="3">
-        <v>10.1</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="B6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="E6" t="s">
         <v>331</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>332</v>
-      </c>
-      <c r="B6" t="s">
-        <v>319</v>
-      </c>
-      <c r="C6" t="s">
-        <v>332</v>
-      </c>
-      <c r="D6" t="s">
-        <v>338</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="F6" s="5">
-        <v>1.2</v>
-      </c>
-      <c r="G6" t="s">
-        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -1943,12 +1893,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCB3A8AA-93BA-4934-8358-CA4D572AC14B}">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="O13" sqref="O13"/>
-      <selection pane="bottomLeft" activeCell="D59" sqref="D59"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1967,490 +1917,482 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>271</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
-        <v>315</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>286</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>286</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B21" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B28" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B35" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B36" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B37" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B38" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B39" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B40" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B41" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B42" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B43" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B44" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B45" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B46" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B47" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B48" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B49" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B50" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B51" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B52" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B53" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B54" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>142</v>
+        <v>333</v>
       </c>
       <c r="B55" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>337</v>
+        <v>287</v>
       </c>
       <c r="B56" t="s">
-        <v>144</v>
+        <v>288</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>287</v>
+        <v>313</v>
       </c>
       <c r="B57" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B58" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>312</v>
+        <v>289</v>
       </c>
       <c r="B59" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B60" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>290</v>
+        <v>330</v>
       </c>
       <c r="B61" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" t="s">
-        <v>332</v>
-      </c>
-      <c r="B62" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -2463,11 +2405,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{891049CA-D2B3-4DE1-AA0F-3009AC7CEAB2}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2486,282 +2428,274 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>271</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>316</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>292</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>303</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B24" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B25" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B26" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B27" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B28" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B29" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B30" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B31" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B32" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B33" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>302</v>
+        <v>335</v>
       </c>
       <c r="B34" t="s">
-        <v>291</v>
+        <v>314</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B35" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" t="s">
-        <v>338</v>
-      </c>
-      <c r="B36" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fixes - code and example data
</commit_message>
<xml_diff>
--- a/hospitalConfig/hospitals/hospital1.xlsx
+++ b/hospitalConfig/hospitals/hospital1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/82cfe7acc6d68563/Documents/github/Clinical-Costing/hospitalConfig/hospitals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="371" documentId="8_{F21D1F19-B0D4-4D89-B817-A6C872BD26CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BC7C6F0-B4F9-4228-8507-B011FA931FE4}"/>
+  <xr:revisionPtr revIDLastSave="373" documentId="8_{F21D1F19-B0D4-4D89-B817-A6C872BD26CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4581593E-133A-4659-BF05-F3988BBB9CBF}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" firstSheet="2" activeTab="10" xr2:uid="{EE86B12F-8EEC-43A3-B99E-E677A24C294A}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" firstSheet="2" activeTab="3" xr2:uid="{EE86B12F-8EEC-43A3-B99E-E677A24C294A}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
@@ -27,7 +27,7 @@
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="2" hidden="1">departments!$A$1:$B$61</definedName>
-    <definedName name="ExternalData_2" localSheetId="3" hidden="1">'cost types'!$A$1:$B$35</definedName>
+    <definedName name="ExternalData_2" localSheetId="3" hidden="1">'cost types'!$A$1:$B$36</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="347">
   <si>
     <t>ADMIN</t>
   </si>
@@ -1096,6 +1096,12 @@
   </si>
   <si>
     <t>Prosthetic Expenses</t>
+  </si>
+  <si>
+    <t>invoiceVariance</t>
+  </si>
+  <si>
+    <t>Variance between invoices and GL account</t>
   </si>
 </sst>
 </file>
@@ -1174,7 +1180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1183,6 +1189,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1251,8 +1258,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{49776610-1554-4112-BBD4-DBCAB5DF817C}" name="costtype" displayName="costtype" ref="A1:B35" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:B35" xr:uid="{49776610-1554-4112-BBD4-DBCAB5DF817C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{49776610-1554-4112-BBD4-DBCAB5DF817C}" name="costtype" displayName="costtype" ref="A1:B36" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:B36" xr:uid="{49776610-1554-4112-BBD4-DBCAB5DF817C}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{D3124862-DA24-43F5-BD00-523AC2BF7B5C}" uniqueName="1" name="cost_type_code" queryTableFieldId="1" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{56F2815C-D89C-4975-A98A-3B9679A67317}" uniqueName="2" name="cost_type_description" queryTableFieldId="2" dataDxfId="0"/>
@@ -1755,7 +1762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2057FB1-CD68-4671-BA7D-809E4713A0D4}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
@@ -2426,11 +2433,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{891049CA-D2B3-4DE1-AA0F-3009AC7CEAB2}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2717,6 +2724,14 @@
       </c>
       <c r="B35" t="s">
         <v>342</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made hospital_code part of model table primary key
</commit_message>
<xml_diff>
--- a/hospitalConfig/hospitals/hospital1.xlsx
+++ b/hospitalConfig/hospitals/hospital1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/82cfe7acc6d68563/Documents/github/Clinical-Costing/hospitalConfig/hospitals/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\russe\OneDrive\Documents\github\Clinical-Costing\hospitalConfig\hospitals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="373" documentId="8_{F21D1F19-B0D4-4D89-B817-A6C872BD26CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4581593E-133A-4659-BF05-F3988BBB9CBF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2125CFC0-2753-4C13-B464-E9566C2E3CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" firstSheet="2" activeTab="3" xr2:uid="{EE86B12F-8EEC-43A3-B99E-E677A24C294A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="2" activeTab="3" xr2:uid="{EE86B12F-8EEC-43A3-B99E-E677A24C294A}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
@@ -1180,7 +1180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1189,7 +1189,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1218,10 +1217,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1269,9 +1264,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1309,7 +1304,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1415,7 +1410,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1557,7 +1552,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1572,139 +1567,139 @@
       <selection pane="bottomLeft" activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>191</v>
       </c>
@@ -1723,13 +1718,13 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.1015625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>315</v>
       </c>
@@ -1737,7 +1732,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>317</v>
       </c>
@@ -1745,7 +1740,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>319</v>
       </c>
@@ -1767,15 +1762,15 @@
       <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.05078125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.5234375" customWidth="1"/>
-    <col min="5" max="5" width="29.7890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.54296875" customWidth="1"/>
+    <col min="5" max="5" width="29.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>321</v>
       </c>
@@ -1792,7 +1787,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>323</v>
       </c>
@@ -1809,7 +1804,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>331</v>
       </c>
@@ -1826,7 +1821,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>325</v>
       </c>
@@ -1843,7 +1838,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>327</v>
       </c>
@@ -1860,7 +1855,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>329</v>
       </c>
@@ -1892,13 +1887,13 @@
       <selection pane="bottomLeft" activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>149</v>
       </c>
@@ -1906,7 +1901,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>151</v>
       </c>
@@ -1929,13 +1924,13 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.734375" customWidth="1"/>
-    <col min="2" max="2" width="27.578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" customWidth="1"/>
+    <col min="2" max="2" width="27.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>145</v>
       </c>
@@ -1943,7 +1938,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>165</v>
       </c>
@@ -1951,7 +1946,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1959,7 +1954,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>286</v>
       </c>
@@ -1967,7 +1962,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -1975,7 +1970,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1983,7 +1978,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -1991,7 +1986,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -1999,7 +1994,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -2007,7 +2002,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -2015,7 +2010,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -2023,7 +2018,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -2031,7 +2026,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -2039,7 +2034,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -2047,7 +2042,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -2055,7 +2050,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -2063,7 +2058,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -2071,7 +2066,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -2079,7 +2074,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -2087,7 +2082,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -2095,7 +2090,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>77</v>
       </c>
@@ -2103,7 +2098,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -2111,7 +2106,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -2119,7 +2114,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>83</v>
       </c>
@@ -2127,7 +2122,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>85</v>
       </c>
@@ -2135,7 +2130,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>87</v>
       </c>
@@ -2143,7 +2138,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>89</v>
       </c>
@@ -2151,7 +2146,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>91</v>
       </c>
@@ -2159,7 +2154,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>93</v>
       </c>
@@ -2167,7 +2162,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -2175,7 +2170,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>96</v>
       </c>
@@ -2183,7 +2178,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>98</v>
       </c>
@@ -2191,7 +2186,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>100</v>
       </c>
@@ -2199,7 +2194,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>102</v>
       </c>
@@ -2207,7 +2202,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>104</v>
       </c>
@@ -2215,7 +2210,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>106</v>
       </c>
@@ -2223,7 +2218,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>108</v>
       </c>
@@ -2231,7 +2226,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>110</v>
       </c>
@@ -2239,7 +2234,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>112</v>
       </c>
@@ -2247,7 +2242,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>114</v>
       </c>
@@ -2255,7 +2250,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>116</v>
       </c>
@@ -2263,7 +2258,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>118</v>
       </c>
@@ -2271,7 +2266,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>120</v>
       </c>
@@ -2279,7 +2274,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>122</v>
       </c>
@@ -2287,7 +2282,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>124</v>
       </c>
@@ -2295,7 +2290,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>126</v>
       </c>
@@ -2303,7 +2298,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>128</v>
       </c>
@@ -2311,7 +2306,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>130</v>
       </c>
@@ -2319,7 +2314,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>132</v>
       </c>
@@ -2327,7 +2322,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>134</v>
       </c>
@@ -2335,7 +2330,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>136</v>
       </c>
@@ -2343,7 +2338,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>138</v>
       </c>
@@ -2351,7 +2346,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>140</v>
       </c>
@@ -2359,7 +2354,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>142</v>
       </c>
@@ -2367,7 +2362,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>332</v>
       </c>
@@ -2375,7 +2370,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>287</v>
       </c>
@@ -2383,7 +2378,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>313</v>
       </c>
@@ -2391,7 +2386,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>312</v>
       </c>
@@ -2399,7 +2394,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>289</v>
       </c>
@@ -2407,7 +2402,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>290</v>
       </c>
@@ -2415,7 +2410,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>329</v>
       </c>
@@ -2437,16 +2432,16 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
+      <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>147</v>
       </c>
@@ -2454,7 +2449,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2462,7 +2457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2470,7 +2465,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2478,7 +2473,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2486,7 +2481,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2494,7 +2489,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2502,7 +2497,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2510,7 +2505,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -2518,7 +2513,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -2526,7 +2521,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -2534,7 +2529,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2542,7 +2537,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -2550,7 +2545,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -2558,7 +2553,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -2566,7 +2561,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -2574,7 +2569,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -2582,7 +2577,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -2590,7 +2585,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -2598,7 +2593,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -2606,7 +2601,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -2614,7 +2609,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -2622,7 +2617,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>292</v>
       </c>
@@ -2630,7 +2625,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>293</v>
       </c>
@@ -2638,7 +2633,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>294</v>
       </c>
@@ -2646,7 +2641,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>295</v>
       </c>
@@ -2654,7 +2649,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>296</v>
       </c>
@@ -2662,7 +2657,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>297</v>
       </c>
@@ -2670,7 +2665,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>298</v>
       </c>
@@ -2678,7 +2673,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>299</v>
       </c>
@@ -2686,7 +2681,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>300</v>
       </c>
@@ -2694,7 +2689,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>301</v>
       </c>
@@ -2702,7 +2697,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>302</v>
       </c>
@@ -2710,7 +2705,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>334</v>
       </c>
@@ -2718,7 +2713,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>333</v>
       </c>
@@ -2726,11 +2721,11 @@
         <v>342</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="8" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>345</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" t="s">
         <v>346</v>
       </c>
     </row>
@@ -2751,13 +2746,13 @@
       <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.83984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>159</v>
       </c>
@@ -2765,7 +2760,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>161</v>
       </c>
@@ -2773,7 +2768,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>163</v>
       </c>
@@ -2781,7 +2776,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>165</v>
       </c>
@@ -2789,7 +2784,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>167</v>
       </c>
@@ -2797,7 +2792,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>169</v>
       </c>
@@ -2819,13 +2814,13 @@
       <selection pane="bottomLeft" activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>192</v>
       </c>
@@ -2833,7 +2828,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -2841,7 +2836,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -2849,7 +2844,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -2857,7 +2852,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -2865,7 +2860,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>85</v>
       </c>
@@ -2873,7 +2868,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>89</v>
       </c>
@@ -2881,7 +2876,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>96</v>
       </c>
@@ -2889,7 +2884,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>104</v>
       </c>
@@ -2897,7 +2892,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>194</v>
       </c>
@@ -2905,7 +2900,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>195</v>
       </c>
@@ -2913,7 +2908,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>196</v>
       </c>
@@ -2921,7 +2916,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>197</v>
       </c>
@@ -2929,7 +2924,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>136</v>
       </c>
@@ -2951,13 +2946,13 @@
       <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7890625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.89453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>213</v>
       </c>
@@ -2965,7 +2960,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>205</v>
       </c>
@@ -2973,7 +2968,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>206</v>
       </c>
@@ -2981,7 +2976,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -3003,9 +2998,9 @@
       <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>211</v>
       </c>
@@ -3013,7 +3008,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>209</v>
       </c>
@@ -3021,7 +3016,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -3029,7 +3024,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>210</v>
       </c>
@@ -3051,13 +3046,13 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.83984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>242</v>
       </c>
@@ -3065,7 +3060,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>271</v>
       </c>
@@ -3073,7 +3068,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>218</v>
       </c>
@@ -3081,7 +3076,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>219</v>
       </c>
@@ -3089,7 +3084,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>220</v>
       </c>
@@ -3097,7 +3092,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>221</v>
       </c>
@@ -3105,7 +3100,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>222</v>
       </c>
@@ -3113,7 +3108,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>223</v>
       </c>
@@ -3121,7 +3116,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>224</v>
       </c>
@@ -3129,7 +3124,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>225</v>
       </c>
@@ -3137,7 +3132,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>226</v>
       </c>
@@ -3145,7 +3140,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>110</v>
       </c>
@@ -3153,7 +3148,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>227</v>
       </c>
@@ -3161,7 +3156,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>114</v>
       </c>
@@ -3169,7 +3164,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>228</v>
       </c>
@@ -3177,7 +3172,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>229</v>
       </c>
@@ -3185,7 +3180,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>230</v>
       </c>
@@ -3193,7 +3188,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>231</v>
       </c>
@@ -3201,7 +3196,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>232</v>
       </c>
@@ -3209,7 +3204,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>233</v>
       </c>
@@ -3217,7 +3212,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>234</v>
       </c>
@@ -3225,7 +3220,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>235</v>
       </c>
@@ -3233,7 +3228,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>236</v>
       </c>
@@ -3241,7 +3236,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>237</v>
       </c>
@@ -3249,7 +3244,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>238</v>
       </c>
@@ -3257,7 +3252,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>239</v>
       </c>
@@ -3265,7 +3260,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>240</v>
       </c>
@@ -3273,7 +3268,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>241</v>
       </c>
@@ -3281,7 +3276,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>272</v>
       </c>
@@ -3289,7 +3284,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>273</v>
       </c>
@@ -3297,7 +3292,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>274</v>
       </c>
@@ -3305,7 +3300,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>275</v>
       </c>
@@ -3313,7 +3308,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>276</v>
       </c>
@@ -3321,7 +3316,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>277</v>
       </c>
@@ -3329,7 +3324,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>278</v>
       </c>

</xml_diff>